<commit_message>
copied mainboard KiCad files
</commit_message>
<xml_diff>
--- a/hardware/pins.xlsx
+++ b/hardware/pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shurik\Dropbox\Robotics\yozh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shuri\Dropbox\Robotics\github\yozh\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23554E2-E3FE-4715-BEFE-F60430014378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596F6F78-D276-4E43-954F-6AAF05B63411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1944" windowWidth="17280" windowHeight="8964" xr2:uid="{2592871D-5CB4-45BA-AF33-93636A88B9F2}"/>
+    <workbookView xWindow="3450" yWindow="540" windowWidth="14400" windowHeight="7360" xr2:uid="{2592871D-5CB4-45BA-AF33-93636A88B9F2}"/>
   </bookViews>
   <sheets>
     <sheet name="V1.1" sheetId="2" r:id="rId1"/>
@@ -198,12 +198,6 @@
     <t>SERVO2</t>
   </si>
   <si>
-    <t>ENC1A</t>
-  </si>
-  <si>
-    <t>ENC1B</t>
-  </si>
-  <si>
     <t>SDA1</t>
   </si>
   <si>
@@ -222,12 +216,6 @@
     <t>MOTOR2B</t>
   </si>
   <si>
-    <t>ENC2B</t>
-  </si>
-  <si>
-    <t>ENC2A</t>
-  </si>
-  <si>
     <t>D-</t>
   </si>
   <si>
@@ -355,6 +343,18 @@
   </si>
   <si>
     <t xml:space="preserve">In code, one can use arduino pin numbers or aliases, obtained by adding PIN_ to signal name. E.g. analogRead(1) is same as analogRead(PIN_ANALOG1). </t>
+  </si>
+  <si>
+    <t>ENC1_SPEED</t>
+  </si>
+  <si>
+    <t>ENC1_DIR</t>
+  </si>
+  <si>
+    <t>ENC2_DIR</t>
+  </si>
+  <si>
+    <t>ENC2_SPEED</t>
   </si>
 </sst>
 </file>
@@ -891,56 +891,56 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="8.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
     </row>
-    <row r="2" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -951,13 +951,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -968,13 +968,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -985,13 +985,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>4</v>
       </c>
@@ -1002,7 +1002,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>6</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>7</v>
       </c>
@@ -1039,13 +1039,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>8</v>
       </c>
@@ -1056,13 +1056,13 @@
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>9</v>
       </c>
@@ -1073,13 +1073,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>10</v>
       </c>
@@ -1090,13 +1090,13 @@
         <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>11</v>
       </c>
@@ -1107,13 +1107,13 @@
         <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>12</v>
       </c>
@@ -1124,13 +1124,13 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>13</v>
       </c>
@@ -1141,13 +1141,13 @@
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>14</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>15</v>
       </c>
@@ -1169,13 +1169,13 @@
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>16</v>
       </c>
@@ -1186,13 +1186,13 @@
         <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>18</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>19</v>
       </c>
@@ -1229,7 +1229,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>20</v>
       </c>
@@ -1241,10 +1241,10 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>21</v>
       </c>
@@ -1255,16 +1255,16 @@
         <v>11</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>22</v>
       </c>
@@ -1275,14 +1275,14 @@
         <v>12</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F25" s="19"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>23</v>
       </c>
@@ -1293,13 +1293,13 @@
         <v>16</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>24</v>
       </c>
@@ -1310,13 +1310,13 @@
         <v>15</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>25</v>
       </c>
@@ -1327,16 +1327,16 @@
         <v>13</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -1347,14 +1347,14 @@
         <v>14</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -1365,13 +1365,13 @@
         <v>17</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>28</v>
       </c>
@@ -1382,13 +1382,13 @@
         <v>18</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>29</v>
       </c>
@@ -1399,13 +1399,13 @@
         <v>19</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>30</v>
       </c>
@@ -1416,13 +1416,13 @@
         <v>20</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -1433,13 +1433,13 @@
         <v>21</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>32</v>
       </c>
@@ -1450,13 +1450,13 @@
         <v>22</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>33</v>
       </c>
@@ -1467,13 +1467,13 @@
         <v>23</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>34</v>
       </c>
@@ -1484,13 +1484,13 @@
         <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>35</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>36</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>37</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>38</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>39</v>
       </c>
@@ -1549,20 +1549,20 @@
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>40</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>41</v>
       </c>
@@ -1573,7 +1573,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>42</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>43</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>44</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>45</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>46</v>
       </c>
@@ -1635,10 +1635,10 @@
       <c r="C49" s="9"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>47</v>
       </c>
@@ -1649,13 +1649,13 @@
         <v>0</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>48</v>
       </c>

</xml_diff>